<commit_message>
code run-time speed improvement
1. Use fft with zero padding to speed up calculation
2. pre-allocate memory to speed up (most of the improvement)
</commit_message>
<xml_diff>
--- a/HW2/Range Migration vs Resolution.xlsx
+++ b/HW2/Range Migration vs Resolution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Radar_Imaging_Class\HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F26493-7412-4AF4-B29F-559EBDCD3844}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A382347-43CD-49D6-9368-8CF7CB7CEA5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>c</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Operation Frequency (GHz)</t>
+  </si>
+  <si>
+    <t>Range Migration</t>
+  </si>
+  <si>
+    <t>Range Resolution</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,7 +414,8 @@
     <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="27.21875" style="1" bestFit="1" customWidth="1"/>
@@ -438,71 +445,82 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>1000</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>30</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>100</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>100</v>
       </c>
-      <c r="E5" s="1">
-        <f>A5*B5*C5*0.000001</f>
+      <c r="E6" s="1">
+        <f>A6*B6*C6*0.000001</f>
         <v>3</v>
       </c>
-      <c r="F5" s="2">
-        <f>$B$1/(2*D5*1000000)</f>
+      <c r="F6" s="2">
+        <f>$B$1/(2*D6*1000000)</f>
         <v>1.5</v>
       </c>
-      <c r="G5" s="2">
-        <f>E5-F5</f>
+      <c r="G6" s="2">
+        <f>E6-F6</f>
         <v>1.5</v>
       </c>
-      <c r="I5" s="2">
-        <f>B1/(B2*1000000000)/4/(C5*0.000001)</f>
+      <c r="I6" s="2">
+        <f>B1/(B2*1000000000)/4/(C6*0.000001)</f>
         <v>75</v>
       </c>
-      <c r="J5" s="2">
-        <f>B1*C5*0.000001/2</f>
+      <c r="J6" s="2">
+        <f>B1*C6*0.000001/2</f>
         <v>15000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I7" s="2"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>